<commit_message>
update with dardenne plots
</commit_message>
<xml_diff>
--- a/Domenique/paper plots (final)/Dardenne.xlsx
+++ b/Domenique/paper plots (final)/Dardenne.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="345" windowWidth="19200" windowHeight="6953"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="19200" windowHeight="6953"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -480,6 +480,12 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>313</v>
+      </c>
+      <c r="B2" s="1">
+        <v>257</v>
+      </c>
       <c r="C2" s="1">
         <v>6.9080000000000004</v>
       </c>
@@ -509,6 +515,12 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>313</v>
+      </c>
+      <c r="B3" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C3" s="1">
         <v>8.2080000000000002</v>
       </c>
@@ -538,6 +550,12 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>313</v>
+      </c>
+      <c r="B4" s="1">
+        <v>283</v>
+      </c>
       <c r="C4" s="1">
         <v>9.3140000000000001</v>
       </c>
@@ -567,6 +585,12 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>323</v>
+      </c>
+      <c r="B5" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C5" s="1">
         <v>8.2059999999999995</v>
       </c>
@@ -596,6 +620,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>323</v>
+      </c>
+      <c r="B6" s="1">
+        <v>278</v>
+      </c>
       <c r="C6" s="1">
         <v>9.1140000000000008</v>
       </c>
@@ -625,6 +655,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>323</v>
+      </c>
+      <c r="B7" s="1">
+        <v>288</v>
+      </c>
       <c r="C7" s="1">
         <v>10.02</v>
       </c>
@@ -654,6 +690,12 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>326.10000000000002</v>
+      </c>
+      <c r="B8" s="1">
+        <v>257</v>
+      </c>
       <c r="C8" s="1">
         <v>7.31</v>
       </c>
@@ -683,6 +725,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>330</v>
+      </c>
+      <c r="B9" s="1">
+        <v>271.2</v>
+      </c>
       <c r="C9" s="1">
         <v>9.0090000000000003</v>
       </c>
@@ -712,6 +760,12 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>332</v>
+      </c>
+      <c r="B10" s="1">
+        <v>283</v>
+      </c>
       <c r="C10" s="1">
         <v>9.9169999999999998</v>
       </c>
@@ -741,6 +795,12 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>296</v>
+      </c>
+      <c r="B11" s="1">
+        <v>257</v>
+      </c>
       <c r="C11" s="1">
         <v>6.4020000000000001</v>
       </c>
@@ -770,6 +830,12 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>313</v>
+      </c>
+      <c r="B12" s="1">
+        <v>257</v>
+      </c>
       <c r="C12" s="1">
         <v>6.6070000000000002</v>
       </c>
@@ -799,6 +865,12 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>313</v>
+      </c>
+      <c r="B13" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C13" s="1">
         <v>8.0090000000000003</v>
       </c>
@@ -828,6 +900,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>323</v>
+      </c>
+      <c r="B14" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C14" s="1">
         <v>8.2129999999999992</v>
       </c>
@@ -857,6 +935,12 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>323</v>
+      </c>
+      <c r="B15" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C15" s="1">
         <v>8.2110000000000003</v>
       </c>
@@ -886,6 +970,12 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>323.10000000000002</v>
+      </c>
+      <c r="B16" s="1">
+        <v>278</v>
+      </c>
       <c r="C16" s="1">
         <v>9.1159999999999997</v>
       </c>
@@ -914,7 +1004,13 @@
         <v>0.94430000000000003</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>326</v>
+      </c>
+      <c r="B17" s="1">
+        <v>257</v>
+      </c>
       <c r="C17" s="1">
         <v>7.8079999999999998</v>
       </c>
@@ -943,7 +1039,13 @@
         <v>0.86180000000000001</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>328</v>
+      </c>
+      <c r="B18" s="1">
+        <v>251.8</v>
+      </c>
       <c r="C18" s="1">
         <v>6.4059999999999997</v>
       </c>
@@ -972,7 +1074,13 @@
         <v>0.83660000000000001</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>333</v>
+      </c>
+      <c r="B19" s="1">
+        <v>257</v>
+      </c>
       <c r="C19" s="1">
         <v>8.1110000000000007</v>
       </c>
@@ -1001,7 +1109,13 @@
         <v>0.85389999999999999</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>333.1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C20" s="1">
         <v>9.1080000000000005</v>
       </c>
@@ -1030,7 +1144,13 @@
         <v>0.89690000000000003</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>340</v>
+      </c>
+      <c r="B21" s="1">
+        <v>263</v>
+      </c>
       <c r="C21" s="1">
         <v>8.7119999999999997</v>
       </c>
@@ -1059,7 +1179,13 @@
         <v>0.87080000000000002</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>340</v>
+      </c>
+      <c r="B22" s="1">
+        <v>273.2</v>
+      </c>
       <c r="C22" s="1">
         <v>9.7110000000000003</v>
       </c>
@@ -1088,7 +1214,13 @@
         <v>0.9052</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>340</v>
+      </c>
+      <c r="B23" s="1">
+        <v>285.10000000000002</v>
+      </c>
       <c r="C23" s="1">
         <v>10.02</v>
       </c>
@@ -1117,7 +1249,13 @@
         <v>0.94079999999999997</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>296</v>
+      </c>
+      <c r="B24" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C24" s="1">
         <v>4.5019999999999998</v>
       </c>
@@ -1146,7 +1284,13 @@
         <v>0.88549999999999995</v>
       </c>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>296</v>
+      </c>
+      <c r="B25" s="1">
+        <v>257</v>
+      </c>
       <c r="C25" s="1">
         <v>6.4</v>
       </c>
@@ -1175,7 +1319,13 @@
         <v>0.9234</v>
       </c>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>313</v>
+      </c>
+      <c r="B26" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C26" s="1">
         <v>5.9</v>
       </c>
@@ -1204,7 +1354,13 @@
         <v>0.86060000000000003</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>313</v>
+      </c>
+      <c r="B27" s="1">
+        <v>257</v>
+      </c>
       <c r="C27" s="1">
         <v>7.4020000000000001</v>
       </c>
@@ -1233,7 +1389,13 @@
         <v>0.89880000000000004</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>313</v>
+      </c>
+      <c r="B28" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C28" s="1">
         <v>8.1150000000000002</v>
       </c>
@@ -1262,7 +1424,13 @@
         <v>0.94540000000000002</v>
       </c>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>323</v>
+      </c>
+      <c r="B29" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C29" s="1">
         <v>6.109</v>
       </c>
@@ -1291,7 +1459,13 @@
         <v>0.84809999999999997</v>
       </c>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>323</v>
+      </c>
+      <c r="B30" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C30" s="1">
         <v>8.4149999999999991</v>
       </c>
@@ -1320,7 +1494,13 @@
         <v>0.92330000000000001</v>
       </c>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>323</v>
+      </c>
+      <c r="B31" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C31" s="1">
         <v>8.2110000000000003</v>
       </c>
@@ -1349,7 +1529,13 @@
         <v>0.92490000000000006</v>
       </c>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>323.10000000000002</v>
+      </c>
+      <c r="B32" s="1">
+        <v>278</v>
+      </c>
       <c r="C32" s="1">
         <v>9.016</v>
       </c>
@@ -1378,7 +1564,13 @@
         <v>0.96609999999999996</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>326</v>
+      </c>
+      <c r="B33" s="1">
+        <v>257</v>
+      </c>
       <c r="C33" s="1">
         <v>8.0129999999999999</v>
       </c>
@@ -1407,7 +1599,13 @@
         <v>0.88149999999999995</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>331.2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>255.1</v>
+      </c>
       <c r="C34" s="1">
         <v>8.4109999999999996</v>
       </c>
@@ -1436,7 +1634,13 @@
         <v>0.86719999999999997</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>333</v>
+      </c>
+      <c r="B35" s="1">
+        <v>257</v>
+      </c>
       <c r="C35" s="1">
         <v>8.7140000000000004</v>
       </c>
@@ -1465,7 +1669,13 @@
         <v>0.87209999999999999</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>333</v>
+      </c>
+      <c r="B36" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C36" s="1">
         <v>8.8179999999999996</v>
       </c>
@@ -1494,7 +1704,13 @@
         <v>0.91849999999999998</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>333</v>
+      </c>
+      <c r="B37" s="1">
+        <v>288</v>
+      </c>
       <c r="C37" s="1">
         <v>10.02</v>
       </c>
@@ -1523,7 +1739,13 @@
         <v>0.97970000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>340</v>
+      </c>
+      <c r="B38" s="1">
+        <v>263</v>
+      </c>
       <c r="C38" s="1">
         <v>8.8130000000000006</v>
       </c>
@@ -1552,7 +1774,13 @@
         <v>0.88959999999999995</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>340</v>
+      </c>
+      <c r="B39" s="1">
+        <v>273.2</v>
+      </c>
       <c r="C39" s="1">
         <v>9.718</v>
       </c>
@@ -1581,7 +1809,13 @@
         <v>0.92469999999999997</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>340</v>
+      </c>
+      <c r="B40" s="1">
+        <v>285.10000000000002</v>
+      </c>
       <c r="C40" s="1">
         <v>9.9179999999999993</v>
       </c>
@@ -1610,7 +1844,13 @@
         <v>0.96120000000000005</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>295.8</v>
+      </c>
+      <c r="B41" s="1">
+        <v>272</v>
+      </c>
       <c r="C41" s="1">
         <v>8.1050000000000004</v>
       </c>
@@ -1639,7 +1879,13 @@
         <v>0.97829999999999995</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
+        <v>296</v>
+      </c>
+      <c r="B42" s="1">
+        <v>257</v>
+      </c>
       <c r="C42" s="1">
         <v>6.6070000000000002</v>
       </c>
@@ -1668,7 +1914,13 @@
         <v>0.93669999999999998</v>
       </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43" s="1">
+        <v>297.2</v>
+      </c>
+      <c r="B43" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C43" s="1">
         <v>6.2030000000000003</v>
       </c>
@@ -1697,7 +1949,13 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="1">
+        <v>313</v>
+      </c>
+      <c r="B44" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C44" s="1">
         <v>7</v>
       </c>
@@ -1726,7 +1984,13 @@
         <v>0.87190000000000001</v>
       </c>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
+        <v>313</v>
+      </c>
+      <c r="B45" s="1">
+        <v>257</v>
+      </c>
       <c r="C45" s="1">
         <v>7.5060000000000002</v>
       </c>
@@ -1755,7 +2019,13 @@
         <v>0.91239999999999999</v>
       </c>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
+        <v>313</v>
+      </c>
+      <c r="B46" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C46" s="1">
         <v>8.3149999999999995</v>
       </c>
@@ -1784,7 +2054,13 @@
         <v>0.95860000000000001</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
+        <v>323</v>
+      </c>
+      <c r="B47" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C47" s="1">
         <v>7.4009999999999998</v>
       </c>
@@ -1813,7 +2089,13 @@
         <v>0.85929999999999995</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48" s="1">
+        <v>323</v>
+      </c>
+      <c r="B48" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C48" s="1">
         <v>8.6159999999999997</v>
       </c>
@@ -1842,7 +2124,13 @@
         <v>0.93779999999999997</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49" s="1">
+        <v>326</v>
+      </c>
+      <c r="B49" s="1">
+        <v>257</v>
+      </c>
       <c r="C49" s="1">
         <v>8.8140000000000001</v>
       </c>
@@ -1871,7 +2159,13 @@
         <v>0.89259999999999995</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
+        <v>327.7</v>
+      </c>
+      <c r="B50" s="1">
+        <v>278</v>
+      </c>
       <c r="C50" s="1">
         <v>10.119999999999999</v>
       </c>
@@ -1900,7 +2194,13 @@
         <v>0.96830000000000005</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51" s="1">
+        <v>333</v>
+      </c>
+      <c r="B51" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C51" s="1">
         <v>9.0180000000000007</v>
       </c>
@@ -1929,7 +2229,13 @@
         <v>0.9304</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A52" s="1">
+        <v>336</v>
+      </c>
+      <c r="B52" s="1">
+        <v>259.3</v>
+      </c>
       <c r="C52" s="1">
         <v>9.3179999999999996</v>
       </c>
@@ -1958,7 +2264,13 @@
         <v>0.88939999999999997</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A53" s="1">
+        <v>336</v>
+      </c>
+      <c r="B53" s="1">
+        <v>273.2</v>
+      </c>
       <c r="C53" s="1">
         <v>9.6189999999999998</v>
       </c>
@@ -1987,7 +2299,13 @@
         <v>0.94269999999999998</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A54" s="1">
+        <v>340</v>
+      </c>
+      <c r="B54" s="1">
+        <v>263</v>
+      </c>
       <c r="C54" s="1">
         <v>9.4179999999999993</v>
       </c>
@@ -2016,7 +2334,13 @@
         <v>0.8992</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A55" s="1">
+        <v>340</v>
+      </c>
+      <c r="B55" s="1">
+        <v>278</v>
+      </c>
       <c r="C55" s="1">
         <v>10.220000000000001</v>
       </c>
@@ -2045,7 +2369,13 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A56" s="1">
+        <v>296.2</v>
+      </c>
+      <c r="B56" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C56" s="1">
         <v>5.5019999999999998</v>
       </c>
@@ -2074,7 +2404,13 @@
         <v>0.90359999999999996</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A57" s="1">
+        <v>313</v>
+      </c>
+      <c r="B57" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C57" s="1">
         <v>7.1020000000000003</v>
       </c>
@@ -2103,7 +2439,13 @@
         <v>0.87890000000000001</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" s="1">
+        <v>313</v>
+      </c>
+      <c r="B58" s="1">
+        <v>257</v>
+      </c>
       <c r="C58" s="1">
         <v>7.3070000000000004</v>
       </c>
@@ -2132,7 +2474,13 @@
         <v>0.9204</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A59" s="1">
+        <v>313</v>
+      </c>
+      <c r="B59" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C59" s="1">
         <v>8.3109999999999999</v>
       </c>
@@ -2161,7 +2509,13 @@
         <v>0.96630000000000005</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A60" s="1">
+        <v>323</v>
+      </c>
+      <c r="B60" s="1">
+        <v>248.2</v>
+      </c>
       <c r="C60" s="1">
         <v>6.61</v>
       </c>
@@ -2190,7 +2544,13 @@
         <v>0.86860000000000004</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A61" s="1">
+        <v>323</v>
+      </c>
+      <c r="B61" s="1">
+        <v>266.39999999999998</v>
+      </c>
       <c r="C61" s="1">
         <v>8.8130000000000006</v>
       </c>
@@ -2219,7 +2579,13 @@
         <v>0.94440000000000002</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" s="1">
+        <v>326</v>
+      </c>
+      <c r="B62" s="1">
+        <v>257</v>
+      </c>
       <c r="C62" s="1">
         <v>8.7080000000000002</v>
       </c>
@@ -2248,7 +2614,13 @@
         <v>0.89980000000000004</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" s="1">
+        <v>333</v>
+      </c>
+      <c r="B63" s="1">
+        <v>257</v>
+      </c>
       <c r="C63" s="1">
         <v>9.0129999999999999</v>
       </c>
@@ -2277,7 +2649,13 @@
         <v>0.89049999999999996</v>
       </c>
     </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A64" s="1">
+        <v>333.1</v>
+      </c>
+      <c r="B64" s="1">
+        <v>268.2</v>
+      </c>
       <c r="C64" s="1">
         <v>9.1110000000000007</v>
       </c>

</xml_diff>